<commit_message>
Updated Generate Report Logic!
</commit_message>
<xml_diff>
--- a/App_Admin/temp/open_question_df.xlsx
+++ b/App_Admin/temp/open_question_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +480,1356 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>109</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Xyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>109</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Abc</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>109</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Uvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>109</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>He should work hard on Django</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>109</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Continue working on the python scripts</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>109</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>He should not stop learning.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>109</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>subhayanroy89@gmail.com</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Continue learning new technology</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>109</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>subhayanroy89@gmail.com</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Be more observant and priotize tasks</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>109</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>subhayanroy89@gmail.com</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Panicking okay</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>109</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ayushsilarpuriaa@gmail.com</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Imagination</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>109</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ayushsilarpuriaa@gmail.com</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Teaching</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>109</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ayushsilarpuriaa@gmail.com</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>109</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>subhayantcpl@gmail.com</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>development</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>109</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>subhayantcpl@gmail.com</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>reading</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>109</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas  J </t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>subhayantcpl@gmail.com</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>writing</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>109</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>109</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>109</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>jafri110world@gmail.com</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>109</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>subhayanroy89@gmail.com</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Continue learning Data Engineering.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>109</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>subhayanroy89@gmail.com</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Start learning guitar.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>109</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>subhayanroy89@gmail.com</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Sing high notes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>109</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Start with GCP certification.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>109</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Work on SQL and python coding</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>109</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Never stop learning</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>109</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>ayushsilarpuriaa@gmail.com</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Learning</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>109</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>ayushsilarpuriaa@gmail.com</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Vibing</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>109</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>ayushsilarpuriaa@gmail.com</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Working</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>109</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>subhayantcpl@gmail.com</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>all good</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>109</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>subhayantcpl@gmail.com</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>all good</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>109</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Anantara_Analytics</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>NeuCode</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Uthsavi  K</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>uthsavi@outlook.com</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>subhayantcpl@gmail.com</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>all good 244</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes: SuperUser Excel file for export status
</commit_message>
<xml_diff>
--- a/App_Admin/temp/open_question_df.xlsx
+++ b/App_Admin/temp/open_question_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,22 +496,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ayush </t>
+          <t xml:space="preserve">Abbas </t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ayush_s@anantsol.com</t>
+          <t>abbas_j@anantsol.com</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>subhayan_r@anantsol.com</t>
+          <t>uthsavi_k@anantsol.com</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Supervisor</t>
+          <t>Peer</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>uu</t>
+          <t>a</t>
         </is>
       </c>
     </row>
@@ -541,22 +541,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ayush </t>
+          <t xml:space="preserve">Abbas </t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ayush_s@anantsol.com</t>
+          <t>abbas_j@anantsol.com</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>subhayan_r@anantsol.com</t>
+          <t>uthsavi_k@anantsol.com</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Supervisor</t>
+          <t>Peer</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -566,7 +566,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>vv</t>
+          <t>b</t>
         </is>
       </c>
     </row>
@@ -586,22 +586,22 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ayush </t>
+          <t xml:space="preserve">Abbas </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ayush_s@anantsol.com</t>
+          <t>abbas_j@anantsol.com</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>subhayan_r@anantsol.com</t>
+          <t>uthsavi_k@anantsol.com</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Supervisor</t>
+          <t>Peer</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>zz</t>
+          <t>c</t>
         </is>
       </c>
     </row>
@@ -631,22 +631,22 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ayush </t>
+          <t xml:space="preserve">Abbas </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>ayush_s@anantsol.com</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>ayush_s@anantsol.com</t>
-        </is>
-      </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Self</t>
+          <t>Peer</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -656,7 +656,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>aaabb</t>
+          <t>Learning...!!</t>
         </is>
       </c>
     </row>
@@ -676,22 +676,22 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ayush </t>
+          <t xml:space="preserve">Abbas </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>ayush_s@anantsol.com</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>ayush_s@anantsol.com</t>
-        </is>
-      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Self</t>
+          <t>Peer</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>bbbaa</t>
+          <t>Teaching...!!</t>
         </is>
       </c>
     </row>
@@ -721,32 +721,1517 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t xml:space="preserve">Abbas </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Overwork...!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>114</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas </t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>subhayan_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>xxyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>114</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas </t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>subhayan_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>yyzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>114</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas </t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>subhayan_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>zzyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>114</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas </t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>good</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>114</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas </t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>good good</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>114</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas </t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>good good good</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>114</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas </t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>barani_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>vhufe</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>114</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>barani_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>bfjkwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>114</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abbas </t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>abbas_j@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>barani_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>wdgjegjnjkengjwjgek</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>114</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t xml:space="preserve">Ayush </t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>ayush_s@anantsol.com</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>barani_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>testing1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>114</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ayush </t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>ayush_s@anantsol.com</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>barani_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>test 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>114</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ayush </t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>barani_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>test test test 33</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>114</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ayush </t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>subhayan_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>uu</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>114</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ayush </t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>subhayan_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>vv</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>114</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ayush </t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>subhayan_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>zz</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>114</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ayush </t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
         <is>
           <t>Self</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>aaabb</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>114</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ayush </t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>bbbaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>114</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ayush </t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
         <is>
           <t>What do you suggest he/she STOP doing?</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>cccdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>114</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ayush </t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>114</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ayush </t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>114</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ayush </t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>114</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uthsavi </t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Learning...!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>114</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uthsavi </t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Teaching...!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>114</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uthsavi </t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>ayush_s@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Peer</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Overwork...!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>114</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uthsavi </t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>barani_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>suggest he/she CONTINUE</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>114</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uthsavi </t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>barani_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>suggest he/she CONTINUE</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>114</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uthsavi </t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>barani_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>suggest he/she CONTINUE</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>114</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uthsavi </t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>subhayan_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Fighting with Abbas</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>114</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uthsavi </t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>subhayan_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Get Starlink from SpaceX</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>114</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uthsavi </t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>subhayan_r@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Saying Oh God! while not sharing screen to scare me</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>114</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uthsavi </t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she CONTINUE doing?</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>114</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uthsavi </t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she START doing?</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>114</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Anantara</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uthsavi </t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>uthsavi_k@anantsol.com</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Self</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>What do you suggest he/she STOP doing?</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>z</t>
         </is>
       </c>
     </row>

</xml_diff>